<commit_message>
*Unstable* Created groupregister.py Added utility functions and override some default functions in Student, Group and GroupRegister
</commit_message>
<xml_diff>
--- a/Skjema uten navn(1-3).xlsx
+++ b/Skjema uten navn(1-3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magnus Brevik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrem\WebstormProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAFF458-998D-4D5E-82E9-A722B606282F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568726D1-0FD6-4FB4-B740-C0D42CFF095E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -51,37 +51,145 @@
     <t>Ønskede samarbeidspartnere? Separer med komma(,) eller semikolon(;)</t>
   </si>
   <si>
-    <t>magbre@ntnu.no</t>
-  </si>
-  <si>
-    <t>Magnus Brevik</t>
-  </si>
-  <si>
     <t>Erfaring med JavaScript;Erfaring med andre språk;</t>
   </si>
   <si>
     <t>Fleksibel</t>
   </si>
   <si>
-    <t>Gloria Treider</t>
-  </si>
-  <si>
     <t>Ingen programmeringserfaring;</t>
   </si>
   <si>
     <t>Dagtid</t>
   </si>
   <si>
-    <t>gloria@ntnu.no</t>
-  </si>
-  <si>
-    <t>test@ntnu.no</t>
-  </si>
-  <si>
-    <t>Test Testesen</t>
-  </si>
-  <si>
-    <t>Gloria Treider; Test Testesen</t>
+    <t>1@ntnu.no</t>
+  </si>
+  <si>
+    <t>2@ntnu.no</t>
+  </si>
+  <si>
+    <t>3@ntnu.no</t>
+  </si>
+  <si>
+    <t>std1</t>
+  </si>
+  <si>
+    <t>std2</t>
+  </si>
+  <si>
+    <t>std3</t>
+  </si>
+  <si>
+    <t>std4</t>
+  </si>
+  <si>
+    <t>std5</t>
+  </si>
+  <si>
+    <t>std6</t>
+  </si>
+  <si>
+    <t>std7</t>
+  </si>
+  <si>
+    <t>std8</t>
+  </si>
+  <si>
+    <t>std9</t>
+  </si>
+  <si>
+    <t>std10</t>
+  </si>
+  <si>
+    <t>std11</t>
+  </si>
+  <si>
+    <t>std12</t>
+  </si>
+  <si>
+    <t>std13</t>
+  </si>
+  <si>
+    <t>std14</t>
+  </si>
+  <si>
+    <t>std15</t>
+  </si>
+  <si>
+    <t>std16</t>
+  </si>
+  <si>
+    <t>std17</t>
+  </si>
+  <si>
+    <t>std18</t>
+  </si>
+  <si>
+    <t>std19</t>
+  </si>
+  <si>
+    <t>std20</t>
+  </si>
+  <si>
+    <t>4@ntnu.no</t>
+  </si>
+  <si>
+    <t>5@ntnu.no</t>
+  </si>
+  <si>
+    <t>6@ntnu.no</t>
+  </si>
+  <si>
+    <t>7@ntnu.no</t>
+  </si>
+  <si>
+    <t>8@ntnu.no</t>
+  </si>
+  <si>
+    <t>9@ntnu.no</t>
+  </si>
+  <si>
+    <t>10@ntnu.no</t>
+  </si>
+  <si>
+    <t>11@ntnu.no</t>
+  </si>
+  <si>
+    <t>12@ntnu.no</t>
+  </si>
+  <si>
+    <t>13@ntnu.no</t>
+  </si>
+  <si>
+    <t>14@ntnu.no</t>
+  </si>
+  <si>
+    <t>15@ntnu.no</t>
+  </si>
+  <si>
+    <t>16@ntnu.no</t>
+  </si>
+  <si>
+    <t>17@ntnu.no</t>
+  </si>
+  <si>
+    <t>18@ntnu.no</t>
+  </si>
+  <si>
+    <t>19@ntnu.no</t>
+  </si>
+  <si>
+    <t>20@ntnu.no</t>
+  </si>
+  <si>
+    <t>Kveldstid</t>
+  </si>
+  <si>
+    <t>std6;std7</t>
+  </si>
+  <si>
+    <t>sgfdhgh</t>
   </si>
 </sst>
 </file>
@@ -89,9 +197,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +211,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,11 +246,11 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -156,10 +270,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -178,8 +292,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H4" totalsRowShown="0">
-  <autoFilter ref="A1:H4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0">
+  <autoFilter ref="A1:H21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Starttidspunkt" dataDxfId="6"/>
@@ -491,21 +605,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.44140625" customWidth="1"/>
     <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -531,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -541,23 +655,23 @@
       <c r="C2" s="2">
         <v>44005.575555555602</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -568,20 +682,22 @@
         <v>44005.576099537</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -592,30 +708,465 @@
         <v>44005.576319444401</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="B16" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44005.57542818287</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44005.575555555559</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{1D575DE4-B2FB-47DD-8B70-CA0B3BC8BD92}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{CC7ECC3B-7258-4F11-8AF5-CD57D70B24CB}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{30512275-B15A-4B18-B150-EBE2084CDDB4}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{5D94167E-FCD6-46CB-A9B9-741F47BE2BDF}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{F469334B-647F-4C1F-BB88-039EB9EA8131}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{11C5BE8B-4730-4EE8-B288-06955C4CD47D}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{CDFE3F9B-208C-4662-9D7A-1AD770EF22E0}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{274882F5-7A69-4B74-AC2A-A671CFDE2975}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{D3B366B4-FDF9-447F-954D-993A44314EA9}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{3764969C-1D5A-46B3-A178-95F9BE25EDA1}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{91EDFFF3-1DA4-4044-ABB4-38BFC638293E}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{7421F476-2BCA-468F-B1C7-7DB9D545343B}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{D9D3F466-71C0-4A4B-9359-D8293269D784}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{93B70405-5BA2-4AF6-A864-E0365E55B3B0}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{88942555-82D5-412A-923F-AD8C7BF05DFC}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{6ECF2EDB-D63E-495C-8B45-E6F8A9011CDA}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{B5B0966C-61A1-44EB-9E21-EB4D2FCBEEC2}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{6DD150DD-CC46-4BA6-A11F-D3DBDD61924D}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{826283D2-624E-45CD-9598-B77B985BCB0B}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{502CDC27-7D36-4030-AA22-EB3D0FDD5881}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added __bool__ override for Group Moved adding of desired partners from GroupRegister to Group Added functionality for removing member from Group Added a time attribute to Group to easily be able to check if the members of the Group mainly desire to work day or night Added function for adding a Student to the GroupRegister Added functionality for combining small groups Added function for moving a Student from a Group to another
</commit_message>
<xml_diff>
--- a/Skjema uten navn(1-3).xlsx
+++ b/Skjema uten navn(1-3).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrem\WebstormProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568726D1-0FD6-4FB4-B740-C0D42CFF095E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473C6B04-20C5-4F86-8BC5-19A0BDE9330E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adds possibility of updating a student with new data If a student answers twice the program will overwrite the values in the old student with the new data Fixed test data. All data _must_ have email, name, programming experience, preferred worktime
</commit_message>
<xml_diff>
--- a/Skjema uten navn(1-3).xlsx
+++ b/Skjema uten navn(1-3).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruker\Documents\SummerStudy\SommerJobb-IDI\idi-project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magnus Brevik\PycharmProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984626D4-E2BC-4952-8F26-A4D1A38909BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42991CAA-F12E-44D8-BAD8-71F32086D028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,33 @@
   </si>
   <si>
     <t>std28</t>
+  </si>
+  <si>
+    <t>21@ntnu.no</t>
+  </si>
+  <si>
+    <t>22@ntnu.no</t>
+  </si>
+  <si>
+    <t>23@ntnu.no</t>
+  </si>
+  <si>
+    <t>24@ntnu.no</t>
+  </si>
+  <si>
+    <t>25@ntnu.no</t>
+  </si>
+  <si>
+    <t>26@ntnu.no</t>
+  </si>
+  <si>
+    <t>27@ntnu.no</t>
+  </si>
+  <si>
+    <t>28@ntnu.no</t>
+  </si>
+  <si>
+    <t>std2;std6</t>
   </si>
 </sst>
 </file>
@@ -274,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -316,8 +343,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H29" totalsRowShown="0">
-  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0">
+  <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Starttidspunkt" dataDxfId="6"/>
@@ -629,21 +656,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.44140625" customWidth="1"/>
+    <col min="6" max="6" width="45.42578125" customWidth="1"/>
     <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -669,7 +696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -695,7 +722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -721,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -745,7 +772,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -769,7 +796,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -795,7 +822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -821,7 +848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -847,7 +874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -871,7 +898,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -895,7 +922,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -921,7 +948,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -945,7 +972,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -971,7 +998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -997,7 +1024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1023,7 +1050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1049,7 +1076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1075,7 +1102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1101,7 +1128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1127,7 +1154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1153,7 +1180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1177,11 +1204,13 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1195,11 +1224,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>56</v>
       </c>
@@ -1213,11 +1244,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E24" s="3" t="s">
         <v>57</v>
       </c>
@@ -1231,11 +1264,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="E25" s="3" t="s">
         <v>58</v>
       </c>
@@ -1249,11 +1284,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E26" s="3" t="s">
         <v>59</v>
       </c>
@@ -1267,11 +1304,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>60</v>
       </c>
@@ -1285,11 +1324,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
+      <c r="D28" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>61</v>
       </c>
@@ -1303,11 +1344,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>62</v>
       </c>
@@ -1319,6 +1362,32 @@
       </c>
       <c r="H29" s="3" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
+        <v>44005.5754282407</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44005.575555555602</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1344,11 +1413,21 @@
     <hyperlink ref="D19" r:id="rId18" xr:uid="{6DD150DD-CC46-4BA6-A11F-D3DBDD61924D}"/>
     <hyperlink ref="D20" r:id="rId19" xr:uid="{826283D2-624E-45CD-9598-B77B985BCB0B}"/>
     <hyperlink ref="D21" r:id="rId20" xr:uid="{502CDC27-7D36-4030-AA22-EB3D0FDD5881}"/>
+    <hyperlink ref="D22:D29" r:id="rId21" display="20@ntnu.no" xr:uid="{C2218DB5-FA37-4270-8E59-16DCE8DD591C}"/>
+    <hyperlink ref="D22" r:id="rId22" xr:uid="{D92A9326-BE73-4CFB-8A0B-0EB680A61D2B}"/>
+    <hyperlink ref="D23" r:id="rId23" xr:uid="{23E1DB53-1770-44B2-AD1C-CBE720D53139}"/>
+    <hyperlink ref="D24" r:id="rId24" xr:uid="{E5E21280-9313-4520-B2A5-CA3D2B027CAC}"/>
+    <hyperlink ref="D25" r:id="rId25" xr:uid="{C5D68A1F-5F55-43FE-8A2A-59326D6715A3}"/>
+    <hyperlink ref="D26" r:id="rId26" xr:uid="{181829DC-9C03-4EA5-A61E-B0A0D49EC2F1}"/>
+    <hyperlink ref="D27" r:id="rId27" xr:uid="{259124A1-39CA-4388-B7B2-5A679D456A03}"/>
+    <hyperlink ref="D28" r:id="rId28" xr:uid="{1E697AEE-F5E7-4CA9-BCE2-FD68E6640359}"/>
+    <hyperlink ref="D29" r:id="rId29" xr:uid="{AD170A3B-7535-453F-9216-BE7F0BB1828B}"/>
+    <hyperlink ref="D30" r:id="rId30" xr:uid="{3391FF0B-C692-4CB9-918D-08AF987CB85E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds buttons for exporting groups and group members as .csv-files formatted for importing in BlackBoard
</commit_message>
<xml_diff>
--- a/Skjema uten navn(1-3).xlsx
+++ b/Skjema uten navn(1-3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magnus Brevik\PycharmProjects\idi-project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrem\WebstormProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42991CAA-F12E-44D8-BAD8-71F32086D028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFC59E-1881-4173-8F8A-2170BC2B3A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -240,7 +240,7 @@
     <t>28@ntnu.no</t>
   </si>
   <si>
-    <t>std2;std6</t>
+    <t>std1 stud1 student1</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -343,8 +343,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0">
-  <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H29" totalsRowShown="0">
+  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Starttidspunkt" dataDxfId="6"/>
@@ -656,21 +656,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.44140625" customWidth="1"/>
     <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -696,7 +696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -710,7 +710,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -722,7 +722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -748,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -772,7 +772,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -796,7 +796,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -822,7 +822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -874,7 +874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -898,7 +898,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -922,7 +922,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -948,7 +948,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -998,7 +998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1224,7 +1224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1244,7 +1244,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1264,7 +1264,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1284,7 +1284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1304,7 +1304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1324,7 +1324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1344,7 +1344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1362,32 +1362,6 @@
       </c>
       <c r="H29" s="3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2">
-        <v>44005.5754282407</v>
-      </c>
-      <c r="C30" s="2">
-        <v>44005.575555555602</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1422,12 +1396,11 @@
     <hyperlink ref="D27" r:id="rId27" xr:uid="{259124A1-39CA-4388-B7B2-5A679D456A03}"/>
     <hyperlink ref="D28" r:id="rId28" xr:uid="{1E697AEE-F5E7-4CA9-BCE2-FD68E6640359}"/>
     <hyperlink ref="D29" r:id="rId29" xr:uid="{AD170A3B-7535-453F-9216-BE7F0BB1828B}"/>
-    <hyperlink ref="D30" r:id="rId30" xr:uid="{3391FF0B-C692-4CB9-918D-08AF987CB85E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test data Now requires username from form
</commit_message>
<xml_diff>
--- a/Skjema uten navn(1-3).xlsx
+++ b/Skjema uten navn(1-3).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrem\WebstormProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFC59E-1881-4173-8F8A-2170BC2B3A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF1A4CD-0D32-4F9A-853D-AA0D8AE76C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -240,7 +240,91 @@
     <t>28@ntnu.no</t>
   </si>
   <si>
-    <t>std1 stud1 student1</t>
+    <t>Brukernavn</t>
+  </si>
+  <si>
+    <t>student1</t>
+  </si>
+  <si>
+    <t>student2</t>
+  </si>
+  <si>
+    <t>student3</t>
+  </si>
+  <si>
+    <t>student4</t>
+  </si>
+  <si>
+    <t>student5</t>
+  </si>
+  <si>
+    <t>student6</t>
+  </si>
+  <si>
+    <t>student7</t>
+  </si>
+  <si>
+    <t>student8</t>
+  </si>
+  <si>
+    <t>student9</t>
+  </si>
+  <si>
+    <t>student10</t>
+  </si>
+  <si>
+    <t>student11</t>
+  </si>
+  <si>
+    <t>student12</t>
+  </si>
+  <si>
+    <t>student13</t>
+  </si>
+  <si>
+    <t>student14</t>
+  </si>
+  <si>
+    <t>student15</t>
+  </si>
+  <si>
+    <t>student16</t>
+  </si>
+  <si>
+    <t>student17</t>
+  </si>
+  <si>
+    <t>student18</t>
+  </si>
+  <si>
+    <t>student19</t>
+  </si>
+  <si>
+    <t>student20</t>
+  </si>
+  <si>
+    <t>student21</t>
+  </si>
+  <si>
+    <t>student22</t>
+  </si>
+  <si>
+    <t>student23</t>
+  </si>
+  <si>
+    <t>student24</t>
+  </si>
+  <si>
+    <t>student25</t>
+  </si>
+  <si>
+    <t>student26</t>
+  </si>
+  <si>
+    <t>student27</t>
+  </si>
+  <si>
+    <t>student28</t>
   </si>
 </sst>
 </file>
@@ -304,7 +388,10 @@
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -343,17 +430,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H29" totalsRowShown="0">
-  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Starttidspunkt" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fullføringstidspunkt" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="E-postadresse" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Navn" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Programmeringserfaring?" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Arbeidstid?" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ønskede samarbeidspartnere? Separer med komma(,) eller semikolon(;)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I29" totalsRowShown="0">
+  <autoFilter ref="A1:I29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Starttidspunkt" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fullføringstidspunkt" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="E-postadresse" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Navn" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{9FCDA347-E786-4CC0-A8BF-82A8DF2920E7}" name="Brukernavn" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Programmeringserfaring?" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Arbeidstid?" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ønskede samarbeidspartnere? Separer med komma(,) eller semikolon(;)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -656,21 +744,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.44140625" customWidth="1"/>
-    <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="45.44140625" customWidth="1"/>
+    <col min="8" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -687,16 +776,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -710,19 +802,22 @@
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -736,19 +831,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -762,17 +860,20 @@
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -786,17 +887,20 @@
         <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -810,19 +914,22 @@
         <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -836,19 +943,22 @@
         <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -862,19 +972,22 @@
         <v>38</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -888,17 +1001,20 @@
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -912,17 +1028,20 @@
         <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -936,19 +1055,22 @@
         <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -962,17 +1084,20 @@
         <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -986,19 +1111,22 @@
         <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1012,19 +1140,22 @@
         <v>44</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1038,19 +1169,22 @@
         <v>45</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1064,19 +1198,22 @@
         <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1090,19 +1227,22 @@
         <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1116,19 +1256,22 @@
         <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1142,19 +1285,22 @@
         <v>49</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1168,19 +1314,22 @@
         <v>50</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1194,17 +1343,20 @@
         <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1212,19 +1364,22 @@
         <v>63</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1232,19 +1387,22 @@
         <v>64</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1252,19 +1410,22 @@
         <v>65</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1272,19 +1433,22 @@
         <v>66</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1292,19 +1456,22 @@
         <v>67</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1312,19 +1479,22 @@
         <v>68</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1332,19 +1502,22 @@
         <v>69</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1352,15 +1525,18 @@
         <v>70</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>